<commit_message>
Fleshed out evaluation section with 200m inst data and some fake data.
</commit_message>
<xml_diff>
--- a/figs_src/data.xlsx
+++ b/figs_src/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" checkCompatibility="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="21720" yWindow="2415" windowWidth="18960" windowHeight="9825" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17475" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="full_mon" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,17 @@
     <sheet name="importance" sheetId="34" r:id="rId27"/>
     <sheet name="importance_graph" sheetId="36" r:id="rId28"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="39">
   <si>
     <t>UMC</t>
   </si>
@@ -174,6 +179,9 @@
   <si>
     <t>anav</t>
   </si>
+  <si>
+    <t>k</t>
+  </si>
 </sst>
 </file>
 
@@ -1056,11 +1064,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151214336"/>
-        <c:axId val="151216128"/>
+        <c:axId val="151148800"/>
+        <c:axId val="151150592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151214336"/>
+        <c:axId val="151148800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1077,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151216128"/>
+        <c:crossAx val="151150592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1077,7 +1085,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151216128"/>
+        <c:axId val="151150592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1116,7 +1124,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151214336"/>
+        <c:crossAx val="151148800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1128,9 +1136,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0"/>
-          <c:y val="0.58229016528192756"/>
-          <c:w val="0.99808622098581845"/>
-          <c:h val="0.20764423746234142"/>
+          <c:y val="0.58229016528192801"/>
+          <c:w val="0.99808622098581801"/>
+          <c:h val="0.20764423746234101"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1795,6 +1803,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -1906,6 +1921,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2017,6 +2039,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2123,11 +2152,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153622016"/>
-        <c:axId val="153623552"/>
+        <c:axId val="153483136"/>
+        <c:axId val="153484672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153622016"/>
+        <c:axId val="153483136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2138,7 +2167,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
-          <a:bodyPr rot="-2700000" vert="horz" anchor="t" anchorCtr="0"/>
+          <a:bodyPr rot="-2700000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2147,7 +2176,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153623552"/>
+        <c:crossAx val="153484672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2155,7 +2184,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153623552"/>
+        <c:axId val="153484672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2186,7 +2215,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153622016"/>
+        <c:crossAx val="153483136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2197,10 +2226,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14882611278033522"/>
-          <c:y val="0.79994682000536366"/>
-          <c:w val="0.43831508534501418"/>
-          <c:h val="2.7983148170137653E-2"/>
+          <c:x val="0"/>
+          <c:y val="0.66176689687103896"/>
+          <c:w val="1"/>
+          <c:h val="0.11699852617247222"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2219,7 +2248,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="900">
+        <a:defRPr sz="800">
           <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
           <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
         </a:defRPr>
@@ -2855,6 +2884,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2966,6 +3002,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -3072,11 +3115,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153731456"/>
-        <c:axId val="153732992"/>
+        <c:axId val="153727744"/>
+        <c:axId val="153729280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153731456"/>
+        <c:axId val="153727744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3086,7 +3129,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153732992"/>
+        <c:crossAx val="153729280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3094,10 +3137,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153732992"/>
+        <c:axId val="153729280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3125,7 +3169,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153731456"/>
+        <c:crossAx val="153727744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3136,10 +3180,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.3090408304808483E-2"/>
-          <c:y val="0.80003956518501307"/>
-          <c:w val="0.34666881181215076"/>
-          <c:h val="2.7983148170137653E-2"/>
+          <c:x val="4.9999870113339097E-2"/>
+          <c:y val="0.82643159106172848"/>
+          <c:w val="0.89999993505666953"/>
+          <c:h val="8.6117419364908424E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3158,7 +3202,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="900">
+        <a:defRPr sz="800">
           <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
           <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
         </a:defRPr>
@@ -3553,11 +3597,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153808896"/>
-        <c:axId val="153810432"/>
+        <c:axId val="153801088"/>
+        <c:axId val="153802624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153808896"/>
+        <c:axId val="153801088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3566,7 +3610,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="153810432"/>
+        <c:crossAx val="153802624"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3574,7 +3618,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153810432"/>
+        <c:axId val="153802624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.2"/>
@@ -3603,13 +3647,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153808896"/>
+        <c:crossAx val="153801088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3620,8 +3665,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.54704969072480059"/>
-          <c:y val="7.8492777001786279E-2"/>
+          <c:x val="0.54704969072480103"/>
+          <c:y val="7.8492777001786307E-2"/>
           <c:w val="0.41448619867053998"/>
           <c:h val="6.9038261161322403E-2"/>
         </c:manualLayout>
@@ -4067,11 +4112,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="154068864"/>
-        <c:axId val="154070400"/>
+        <c:axId val="153999616"/>
+        <c:axId val="154001408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154068864"/>
+        <c:axId val="153999616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4080,7 +4125,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154070400"/>
+        <c:crossAx val="154001408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4088,7 +4133,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154070400"/>
+        <c:axId val="154001408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4118,7 +4163,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154068864"/>
+        <c:crossAx val="153999616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4946,11 +4991,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151337216"/>
-        <c:axId val="151347200"/>
+        <c:axId val="151329024"/>
+        <c:axId val="151343104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151337216"/>
+        <c:axId val="151329024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4959,7 +5004,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151347200"/>
+        <c:crossAx val="151343104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4967,7 +5012,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151347200"/>
+        <c:axId val="151343104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5006,7 +5051,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151337216"/>
+        <c:crossAx val="151329024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5018,9 +5063,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0"/>
-          <c:y val="0.58769819711400706"/>
-          <c:w val="0.9940944069297839"/>
-          <c:h val="0.20269481598642963"/>
+          <c:y val="0.58769819711400695"/>
+          <c:w val="0.99409440692978401"/>
+          <c:h val="0.20269481598642999"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -6034,11 +6079,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151443712"/>
-        <c:axId val="151453696"/>
+        <c:axId val="151435520"/>
+        <c:axId val="151445504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151443712"/>
+        <c:axId val="151435520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6058,7 +6103,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="151453696"/>
+        <c:crossAx val="151445504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -6066,7 +6111,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151453696"/>
+        <c:axId val="151445504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6085,7 +6130,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>% Checks</a:t>
+                  <a:t>Coverage</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6094,8 +6139,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.4220408001354818E-2"/>
-              <c:y val="0.19083486496831809"/>
+              <c:x val="2.4220408001354801E-2"/>
+              <c:y val="0.190834864968318"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -6104,7 +6149,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151443712"/>
+        <c:crossAx val="151435520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6115,10 +6160,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0"/>
-          <c:y val="0.66886981088174569"/>
-          <c:w val="1"/>
-          <c:h val="7.4683101063924992E-2"/>
+          <c:x val="0.2059114479508368"/>
+          <c:y val="0.8435287366002252"/>
+          <c:w val="0.58817710409832646"/>
+          <c:h val="8.6334289202725775E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -6773,6 +6818,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -6884,6 +6936,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -6995,6 +7054,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -7101,11 +7167,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="152790912"/>
-        <c:axId val="152792448"/>
+        <c:axId val="152717184"/>
+        <c:axId val="152718720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152790912"/>
+        <c:axId val="152717184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7116,7 +7182,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
-          <a:bodyPr rot="-2700000" vert="horz" anchor="t" anchorCtr="0"/>
+          <a:bodyPr rot="-2700000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -7125,7 +7191,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152792448"/>
+        <c:crossAx val="152718720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7133,7 +7199,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152792448"/>
+        <c:axId val="152718720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7152,7 +7218,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>% Checks</a:t>
+                  <a:t>Coverage</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -7164,7 +7230,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152790912"/>
+        <c:crossAx val="152717184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7175,10 +7241,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14882611278033522"/>
-          <c:y val="0.79994682000536366"/>
-          <c:w val="0.43831508534501418"/>
-          <c:h val="2.7983148170137653E-2"/>
+          <c:x val="0.2059114479508368"/>
+          <c:y val="0.8435287366002252"/>
+          <c:w val="0.58817710409832646"/>
+          <c:h val="8.6334289202725775E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -7197,7 +7263,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="900">
+        <a:defRPr sz="800">
           <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
           <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
         </a:defRPr>
@@ -7833,6 +7899,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -7944,6 +8017,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -8050,11 +8130,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="152885120"/>
-        <c:axId val="152886656"/>
+        <c:axId val="151635840"/>
+        <c:axId val="151637376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152885120"/>
+        <c:axId val="151635840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8064,7 +8144,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152886656"/>
+        <c:crossAx val="151637376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8072,10 +8152,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152886656"/>
+        <c:axId val="151637376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -8103,7 +8184,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152885120"/>
+        <c:crossAx val="151635840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8114,10 +8195,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.3090408304808483E-2"/>
-          <c:y val="0.80003956518501307"/>
-          <c:w val="0.34666881181215076"/>
-          <c:h val="2.7983148170137653E-2"/>
+          <c:x val="4.9999870250688645E-2"/>
+          <c:y val="0.84359091315419721"/>
+          <c:w val="0.89999993512534437"/>
+          <c:h val="8.5997721641426703E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -8136,7 +8217,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="900">
+        <a:defRPr sz="800">
           <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
           <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
         </a:defRPr>
@@ -9100,11 +9181,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153056768"/>
-        <c:axId val="153058304"/>
+        <c:axId val="152932352"/>
+        <c:axId val="152933888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153056768"/>
+        <c:axId val="152932352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9124,7 +9205,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153058304"/>
+        <c:crossAx val="152933888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -9132,7 +9213,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153058304"/>
+        <c:axId val="152933888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -9160,8 +9241,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.4220408001354818E-2"/>
-              <c:y val="0.19083486496831809"/>
+              <c:x val="2.4220408001354801E-2"/>
+              <c:y val="0.190834864968318"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -9170,7 +9251,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153056768"/>
+        <c:crossAx val="152932352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9181,10 +9262,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10762282701677622"/>
-          <c:y val="0.8208076323343505"/>
-          <c:w val="0.43831508534501418"/>
-          <c:h val="2.7983148170137653E-2"/>
+          <c:x val="0.107622827016776"/>
+          <c:y val="0.82080763233435095"/>
+          <c:w val="0.43831508534501401"/>
+          <c:h val="2.7983148170137698E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -10167,11 +10248,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153230720"/>
-        <c:axId val="153244800"/>
+        <c:axId val="153083264"/>
+        <c:axId val="153162880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153230720"/>
+        <c:axId val="153083264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10191,7 +10272,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153244800"/>
+        <c:crossAx val="153162880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10199,7 +10280,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153244800"/>
+        <c:axId val="153162880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -10230,7 +10311,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153230720"/>
+        <c:crossAx val="153083264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10241,10 +10322,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14882611278033522"/>
-          <c:y val="0.79994682000536366"/>
-          <c:w val="0.43831508534501418"/>
-          <c:h val="2.7983148170137653E-2"/>
+          <c:x val="0.148826112780335"/>
+          <c:y val="0.79994682000536399"/>
+          <c:w val="0.43831508534501401"/>
+          <c:h val="2.7983148170137698E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -11116,11 +11197,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153323776"/>
-        <c:axId val="153333760"/>
+        <c:axId val="153258240"/>
+        <c:axId val="153268224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153323776"/>
+        <c:axId val="153258240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11130,7 +11211,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153333760"/>
+        <c:crossAx val="153268224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11138,7 +11219,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153333760"/>
+        <c:axId val="153268224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -11169,7 +11250,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153323776"/>
+        <c:crossAx val="153258240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11180,10 +11261,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.3090408304808483E-2"/>
-          <c:y val="0.80003956518501307"/>
-          <c:w val="0.34666881181215076"/>
-          <c:h val="2.7983148170137653E-2"/>
+          <c:x val="9.3090408304808497E-2"/>
+          <c:y val="0.80003956518501296"/>
+          <c:w val="0.34666881181215098"/>
+          <c:h val="2.7983148170137698E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -11838,6 +11919,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -11949,6 +12037,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -12060,6 +12155,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -12166,11 +12268,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153511808"/>
-        <c:axId val="153513344"/>
+        <c:axId val="153372544"/>
+        <c:axId val="153374080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153511808"/>
+        <c:axId val="153372544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12185,12 +12287,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900"/>
+              <a:defRPr/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153513344"/>
+        <c:crossAx val="153374080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -12198,7 +12300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153513344"/>
+        <c:axId val="153374080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -12226,8 +12328,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.4220408001354818E-2"/>
-              <c:y val="0.19083486496831809"/>
+              <c:x val="2.4220408001354801E-2"/>
+              <c:y val="0.190834864968318"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -12236,7 +12338,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153511808"/>
+        <c:crossAx val="153372544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12247,10 +12349,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10762282701677622"/>
-          <c:y val="0.8208076323343505"/>
-          <c:w val="0.43831508534501418"/>
-          <c:h val="2.7983148170137653E-2"/>
+          <c:x val="0"/>
+          <c:y val="0.6850547470769851"/>
+          <c:w val="1"/>
+          <c:h val="7.0422825760579802E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -12269,7 +12371,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="900">
+        <a:defRPr sz="800">
           <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
           <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
         </a:defRPr>
@@ -12287,8 +12389,8 @@
     <sheetView zoomScale="200" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
+  <drawing r:id="rId1"/>
 </chartsheet>
 </file>
 
@@ -12296,10 +12398,10 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="224" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </chartsheet>
 </file>
@@ -12308,10 +12410,10 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="223" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </chartsheet>
 </file>
@@ -12320,11 +12422,11 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="400" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="68" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="300" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="300" orientation="landscape" horizontalDpi="1200" verticalDpi="1200"/>
+  <drawing r:id="rId1"/>
 </chartsheet>
 </file>
 
@@ -12347,8 +12449,8 @@
     <sheetView zoomScale="310" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
+  <drawing r:id="rId1"/>
 </chartsheet>
 </file>
 
@@ -12356,10 +12458,10 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="365" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="192" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="159" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </chartsheet>
 </file>
@@ -12368,10 +12470,10 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="192" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="159" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </chartsheet>
 </file>
@@ -12380,10 +12482,10 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="224" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </chartsheet>
 </file>
@@ -12392,11 +12494,11 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="68" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200"/>
+  <drawing r:id="rId1"/>
 </chartsheet>
 </file>
 
@@ -12404,11 +12506,11 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="68" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200"/>
+  <drawing r:id="rId1"/>
 </chartsheet>
 </file>
 
@@ -12416,11 +12518,11 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="68" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200"/>
+  <drawing r:id="rId1"/>
 </chartsheet>
 </file>
 
@@ -12428,10 +12530,10 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="224" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </chartsheet>
 </file>
@@ -12440,7 +12542,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="3081338" cy="2176463"/>
+    <xdr:ext cx="2928938" cy="2024063"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -12467,7 +12569,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9627973" cy="7353986"/>
+    <xdr:ext cx="3082868" cy="2181395"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1"/>
@@ -12494,7 +12596,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9627973" cy="7353986"/>
+    <xdr:ext cx="3079608" cy="2178363"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1"/>
@@ -12521,7 +12623,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="2609850" cy="1264444"/>
+    <xdr:ext cx="9651066" cy="7367868"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -12575,7 +12677,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="3076575" cy="2181225"/>
+    <xdr:ext cx="2925097" cy="2021758"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1"/>
@@ -12602,7 +12704,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="3081925" cy="2179007"/>
+    <xdr:ext cx="6275586" cy="2172891"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -12629,7 +12731,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9627973" cy="7353986"/>
+    <xdr:ext cx="6275586" cy="2172891"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -12656,7 +12758,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9627973" cy="7353986"/>
+    <xdr:ext cx="3082868" cy="2181395"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -12683,7 +12785,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9627973" cy="7353986"/>
+    <xdr:ext cx="9651066" cy="7367868"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1"/>
@@ -12710,7 +12812,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9627973" cy="7353986"/>
+    <xdr:ext cx="9651066" cy="7367868"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1"/>
@@ -12737,7 +12839,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9627973" cy="7353986"/>
+    <xdr:ext cx="9651066" cy="7367868"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1"/>
@@ -12764,7 +12866,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9627973" cy="7353986"/>
+    <xdr:ext cx="3082868" cy="2181395"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1"/>
@@ -13300,7 +13402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -13715,6 +13817,11 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -14094,6 +14201,11 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -14300,7 +14412,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -14515,7 +14627,12 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -14524,7 +14641,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -14725,7 +14842,12 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -14856,7 +14978,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -14867,10 +14989,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -14878,7 +15000,7 @@
     <col min="1" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="B1" s="6" t="s">
         <v>21</v>
       </c>
@@ -14919,7 +15041,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -14963,8 +15085,12 @@
         <f>GEOMEAN(B2:M2)</f>
         <v>4.3970736423760846</v>
       </c>
+      <c r="P2" s="2">
+        <f>0.5/(N2-1)</f>
+        <v>0.14718550512501541</v>
+      </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:16">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -15008,8 +15134,12 @@
         <f t="shared" ref="N3:N4" si="0">GEOMEAN(B3:M3)</f>
         <v>2.9221309676106046</v>
       </c>
+      <c r="P3" s="2">
+        <f>0.5/(N3-1)</f>
+        <v>0.2601279561202578</v>
+      </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -15054,14 +15184,19 @@
         <v>1.1329552766613324</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="2">
-        <v>13</v>
+    <row r="6" spans="1:16">
+      <c r="L6" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -15482,6 +15617,11 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -15489,7 +15629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -16714,6 +16854,11 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -16721,7 +16866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -17136,6 +17281,11 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -17515,6 +17665,11 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -17936,5 +18091,10 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 10% overhead data.
</commit_message>
<xml_diff>
--- a/figs_src/data.xlsx
+++ b/figs_src/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" checkCompatibility="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17475" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17475" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="full_mon" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="45">
   <si>
     <t>UMC</t>
   </si>
@@ -197,6 +197,9 @@
   <si>
     <t>h</t>
   </si>
+  <si>
+    <t>700% Overhead</t>
+  </si>
 </sst>
 </file>
 
@@ -205,8 +208,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0000_);[Red]\(0.0000\)"/>
-    <numFmt numFmtId="167" formatCode="0.0_);[Red]\(0.0\)"/>
-    <numFmt numFmtId="168" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="166" formatCode="0.0_);[Red]\(0.0\)"/>
+    <numFmt numFmtId="167" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -277,15 +280,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -912,11 +915,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="152197376"/>
-        <c:axId val="152199168"/>
+        <c:axId val="155332608"/>
+        <c:axId val="155334144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152197376"/>
+        <c:axId val="155332608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -925,7 +928,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152199168"/>
+        <c:crossAx val="155334144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -933,7 +936,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152199168"/>
+        <c:axId val="155334144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -965,14 +968,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0_);[Red]\(0.0\)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152197376"/>
+        <c:crossAx val="155332608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2000,11 +2002,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153617920"/>
-        <c:axId val="153619456"/>
+        <c:axId val="157786112"/>
+        <c:axId val="157787648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153617920"/>
+        <c:axId val="157786112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2024,7 +2026,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153619456"/>
+        <c:crossAx val="157787648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2032,7 +2034,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153619456"/>
+        <c:axId val="157787648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2062,7 +2064,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153617920"/>
+        <c:crossAx val="157786112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2962,11 +2964,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153731456"/>
-        <c:axId val="153732992"/>
+        <c:axId val="157874816"/>
+        <c:axId val="157884800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153731456"/>
+        <c:axId val="157874816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2976,7 +2978,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153732992"/>
+        <c:crossAx val="157884800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2984,7 +2986,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153732992"/>
+        <c:axId val="157884800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3015,7 +3017,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153731456"/>
+        <c:crossAx val="157874816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3443,11 +3445,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153804800"/>
-        <c:axId val="153806336"/>
+        <c:axId val="157964544"/>
+        <c:axId val="157978624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153804800"/>
+        <c:axId val="157964544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3456,7 +3458,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="153806336"/>
+        <c:crossAx val="157978624"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3464,7 +3466,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153806336"/>
+        <c:axId val="157978624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.2"/>
@@ -3499,7 +3501,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153804800"/>
+        <c:crossAx val="157964544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3957,11 +3959,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="154003328"/>
-        <c:axId val="154004864"/>
+        <c:axId val="158171520"/>
+        <c:axId val="158173056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154003328"/>
+        <c:axId val="158171520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3970,7 +3972,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154004864"/>
+        <c:crossAx val="158173056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3978,7 +3980,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154004864"/>
+        <c:axId val="158173056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4008,7 +4010,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154003328"/>
+        <c:crossAx val="158171520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4662,11 +4664,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="152377600"/>
-        <c:axId val="152391680"/>
+        <c:axId val="155563136"/>
+        <c:axId val="155564672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152377600"/>
+        <c:axId val="155563136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4675,7 +4677,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152391680"/>
+        <c:crossAx val="155564672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4683,7 +4685,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152391680"/>
+        <c:axId val="155564672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4715,14 +4717,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0_);[Red]\(0.0\)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152377600"/>
+        <c:crossAx val="155563136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4806,7 +4807,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>50%</c:v>
+                  <c:v>10%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4864,22 +4865,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.91379999999999995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.53779999999999994</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.75449999999999995</c:v>
+                  <c:v>0.87609999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51449999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70809999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98899999999999999</c:v>
+                  <c:v>0.98219999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.96160000000000001</c:v>
+                  <c:v>0.95250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.58260000000000001</c:v>
+                  <c:v>0.57750000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -4888,10 +4889,10 @@
                   <c:v>0.9819</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.78669999999999995</c:v>
+                  <c:v>0.77080000000000004</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.83421111111111101</c:v>
+                  <c:v>0.81820000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4906,7 +4907,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>100%</c:v>
+                  <c:v>50%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4964,22 +4965,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.94740000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.56659999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.7843</c:v>
+                  <c:v>0.91379999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53779999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75449999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.99690000000000001</c:v>
+                  <c:v>0.98899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.9647</c:v>
+                  <c:v>0.96160000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.59370000000000001</c:v>
+                  <c:v>0.58260000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -4988,10 +4989,10 @@
                   <c:v>0.9819</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.80920000000000003</c:v>
+                  <c:v>0.78669999999999995</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.84941111111111101</c:v>
+                  <c:v>0.83420000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5006,7 +5007,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>200%</c:v>
+                  <c:v>100%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5064,22 +5065,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.98809999999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.61870000000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.84840000000000004</c:v>
+                  <c:v>0.94740000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56659999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7843</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.99690000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.97</c:v>
+                  <c:v>0.9647</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.62849999999999995</c:v>
+                  <c:v>0.59370000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -5088,10 +5089,10 @@
                   <c:v>0.9819</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.84319999999999995</c:v>
+                  <c:v>0.80920000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.87507777777777784</c:v>
+                  <c:v>0.84940000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5106,7 +5107,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>300%</c:v>
+                  <c:v>200%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5164,34 +5165,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.66549999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.89729999999999999</c:v>
+                  <c:v>0.98809999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.61870000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84840000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.997</c:v>
+                  <c:v>0.99690000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.97360000000000002</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.66720000000000002</c:v>
+                  <c:v>0.62849999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.98199999999999998</c:v>
+                  <c:v>0.9819</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.87580000000000002</c:v>
+                  <c:v>0.84319999999999995</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.89537777777777783</c:v>
+                  <c:v>0.87509999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5206,7 +5207,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>400%</c:v>
+                  <c:v>300%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5267,19 +5268,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70620000000000005</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.94279999999999997</c:v>
+                  <c:v>0.66549999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89729999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.97609999999999997</c:v>
+                  <c:v>0.97360000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.65990000000000004</c:v>
+                  <c:v>0.66720000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -5288,10 +5289,10 @@
                   <c:v>0.98199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.89590000000000003</c:v>
+                  <c:v>0.87580000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.90665555555555555</c:v>
+                  <c:v>0.89539999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5306,7 +5307,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>500%</c:v>
+                  <c:v>400%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5367,19 +5368,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.73109999999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.98309999999999997</c:v>
+                  <c:v>0.70620000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94279999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.99709999999999999</c:v>
+                  <c:v>0.997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.97909999999999997</c:v>
+                  <c:v>0.97609999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.66790000000000005</c:v>
+                  <c:v>0.65990000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -5388,10 +5389,10 @@
                   <c:v>0.98199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.95599999999999996</c:v>
+                  <c:v>0.89590000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.92181111111111114</c:v>
+                  <c:v>0.90669999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5406,7 +5407,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>600%</c:v>
+                  <c:v>500%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5467,19 +5468,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.79949999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.73109999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98309999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.99709999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.98119999999999996</c:v>
+                  <c:v>0.97909999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.74819999999999998</c:v>
+                  <c:v>0.66790000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -5488,10 +5489,10 @@
                   <c:v>0.98199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.99439999999999995</c:v>
+                  <c:v>0.95599999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.94471111111111106</c:v>
+                  <c:v>0.92179999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5506,7 +5507,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>700% Overhead</c:v>
+                  <c:v>600%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5567,7 +5568,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.86660000000000004</c:v>
+                  <c:v>0.79949999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -5576,6 +5577,106 @@
                   <c:v>0.99709999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.98119999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74819999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99439999999999995</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.0000">
+                  <c:v>0.94469999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>bc!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>700% Overhead</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>bc!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>perlbench</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bzip2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mcf</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gobmk</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>hmmer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>sjeng</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h264ref</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>bc!$B$10:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.86660000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99709999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.98319999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
@@ -5590,8 +5691,8 @@
                 <c:pt idx="8">
                   <c:v>0.99970000000000003</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.95586666666666664</c:v>
+                <c:pt idx="9">
+                  <c:v>0.95589999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5606,17 +5707,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="152484096"/>
-        <c:axId val="152494080"/>
+        <c:axId val="156783360"/>
+        <c:axId val="156784896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152484096"/>
+        <c:axId val="156783360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5630,7 +5731,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152494080"/>
+        <c:crossAx val="156784896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -5638,7 +5739,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152494080"/>
+        <c:axId val="156784896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -5676,7 +5777,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152484096"/>
+        <c:crossAx val="156783360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5689,8 +5790,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.20591144795083699"/>
           <c:y val="0.84352873660022498"/>
-          <c:w val="0.58817710409832702"/>
-          <c:h val="8.6334289202725706E-2"/>
+          <c:w val="0.6423086850840265"/>
+          <c:h val="8.5941855761350147E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5750,7 +5851,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>50%</c:v>
+                  <c:v>10%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5808,34 +5909,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.43049999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.22689999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.44140000000000001</c:v>
+                  <c:v>0.26540000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10780000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27150000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.82330000000000003</c:v>
+                  <c:v>0.34770000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.39529999999999998</c:v>
+                  <c:v>0.2445</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4148</c:v>
+                  <c:v>0.12690000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.49149999999999999</c:v>
+                  <c:v>0.36809999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.97660000000000002</c:v>
+                  <c:v>0.9587</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.3533</c:v>
+                  <c:v>0.1996</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.5059555555555556</c:v>
+                  <c:v>0.3211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5850,7 +5951,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>100%</c:v>
+                  <c:v>50%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5908,34 +6009,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.55300000000000005</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.32629999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.59430000000000005</c:v>
+                  <c:v>0.43049999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22689999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.44140000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.89680000000000004</c:v>
+                  <c:v>0.82330000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.51849999999999996</c:v>
+                  <c:v>0.39529999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.74660000000000004</c:v>
+                  <c:v>0.4148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59719999999999995</c:v>
+                  <c:v>0.49149999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.99470000000000003</c:v>
+                  <c:v>0.97660000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.47570000000000001</c:v>
+                  <c:v>0.3533</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.63367777777777767</c:v>
+                  <c:v>0.50600000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5950,7 +6051,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>200%</c:v>
+                  <c:v>100%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6008,34 +6109,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.78580000000000005</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.51400000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.81979999999999997</c:v>
+                  <c:v>0.55300000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32629999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59430000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.94910000000000005</c:v>
+                  <c:v>0.89680000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.70230000000000004</c:v>
+                  <c:v>0.51849999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.91339999999999999</c:v>
+                  <c:v>0.74660000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8196</c:v>
+                  <c:v>0.59719999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.99860000000000004</c:v>
+                  <c:v>0.99470000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.71289999999999998</c:v>
+                  <c:v>0.47570000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.80172222222222222</c:v>
+                  <c:v>0.63370000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6050,7 +6151,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>300%</c:v>
+                  <c:v>200%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6108,34 +6209,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.64870000000000005</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.99650000000000005</c:v>
+                  <c:v>0.78580000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.81979999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98370000000000002</c:v>
+                  <c:v>0.94910000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.86770000000000003</c:v>
+                  <c:v>0.70230000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.91339999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.99839999999999995</c:v>
+                  <c:v>0.8196</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.99960000000000004</c:v>
+                  <c:v>0.99860000000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.9284</c:v>
+                  <c:v>0.71289999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.93588888888888888</c:v>
+                  <c:v>0.80169999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6150,7 +6251,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>400%</c:v>
+                  <c:v>300%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6211,31 +6312,31 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.77729999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.64870000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99650000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.99980000000000002</c:v>
+                  <c:v>0.98370000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.86770000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.99919999999999998</c:v>
+                  <c:v>0.99839999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.99980000000000002</c:v>
+                  <c:v>0.99960000000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.9284</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.97512222222222222</c:v>
+                  <c:v>0.93589999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6250,7 +6351,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>500%</c:v>
+                  <c:v>400%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6311,13 +6412,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.91</c:v>
+                  <c:v>0.77729999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.99990000000000001</c:v>
+                  <c:v>0.99980000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -6326,16 +6427,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.99929999999999997</c:v>
+                  <c:v>0.99919999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0.99980000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.98991111111111119</c:v>
+                  <c:v>0.97509999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6350,7 +6451,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>600%</c:v>
+                  <c:v>500%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6411,7 +6512,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99199999999999999</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -6426,7 +6527,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.99939999999999996</c:v>
+                  <c:v>0.99929999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -6435,7 +6536,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.99903333333333322</c:v>
+                  <c:v>0.9899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6450,7 +6551,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>700% Overhead</c:v>
+                  <c:v>600%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6511,13 +6612,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.99199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.99990000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -6535,7 +6636,107 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.99993333333333334</c:v>
+                  <c:v>0.999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>umc!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>700% Overhead</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>umc!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>perlbench</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bzip2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mcf</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gobmk</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>hmmer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>sjeng</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h264ref</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>umc!$B$10:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99939999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99990000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6550,11 +6751,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="152782720"/>
-        <c:axId val="152784256"/>
+        <c:axId val="156971392"/>
+        <c:axId val="156972928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152782720"/>
+        <c:axId val="156971392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6574,7 +6775,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152784256"/>
+        <c:crossAx val="156972928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6582,7 +6783,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152784256"/>
+        <c:axId val="156972928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6613,7 +6814,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152782720"/>
+        <c:crossAx val="156971392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6626,8 +6827,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.20591144795083699"/>
           <c:y val="0.84352873660022498"/>
-          <c:w val="0.58817710409832702"/>
-          <c:h val="8.6334289202725706E-2"/>
+          <c:w val="0.65846255946871091"/>
+          <c:h val="9.2497357147928713E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -7513,11 +7714,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="152749952"/>
-        <c:axId val="152751488"/>
+        <c:axId val="157065600"/>
+        <c:axId val="157067136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152749952"/>
+        <c:axId val="157065600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7527,7 +7728,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152751488"/>
+        <c:crossAx val="157067136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7535,7 +7736,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152751488"/>
+        <c:axId val="157067136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7560,14 +7761,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152749952"/>
+        <c:crossAx val="157065600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8564,11 +8764,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="152991232"/>
-        <c:axId val="152992768"/>
+        <c:axId val="157157632"/>
+        <c:axId val="157175808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152991232"/>
+        <c:axId val="157157632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8588,7 +8788,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152992768"/>
+        <c:crossAx val="157175808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -8596,7 +8796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152992768"/>
+        <c:axId val="157175808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -8634,7 +8834,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152991232"/>
+        <c:crossAx val="157157632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9631,11 +9831,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153148800"/>
-        <c:axId val="153162880"/>
+        <c:axId val="157394816"/>
+        <c:axId val="157396352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153148800"/>
+        <c:axId val="157394816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9655,7 +9855,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153162880"/>
+        <c:crossAx val="157396352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9663,7 +9863,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153162880"/>
+        <c:axId val="157396352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -9693,7 +9893,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153148800"/>
+        <c:crossAx val="157394816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10579,11 +10779,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153258240"/>
-        <c:axId val="153272320"/>
+        <c:axId val="157430528"/>
+        <c:axId val="157432064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153258240"/>
+        <c:axId val="157430528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10593,7 +10793,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153272320"/>
+        <c:crossAx val="157432064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10601,7 +10801,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153272320"/>
+        <c:axId val="157432064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -10631,7 +10831,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153258240"/>
+        <c:crossAx val="157430528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11649,11 +11849,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153438080"/>
-        <c:axId val="153439616"/>
+        <c:axId val="157540736"/>
+        <c:axId val="157542272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153438080"/>
+        <c:axId val="157540736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11673,7 +11873,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153439616"/>
+        <c:crossAx val="157542272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -11681,7 +11881,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153439616"/>
+        <c:axId val="157542272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -11719,7 +11919,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153438080"/>
+        <c:crossAx val="157540736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11839,7 +12039,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="204" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="144" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="159" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -11851,7 +12051,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="204" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="147" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="159" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -12085,7 +12285,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="6279963" cy="2180478"/>
+    <xdr:ext cx="6283854" cy="2182813"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -12112,7 +12312,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="6279963" cy="2180478"/>
+    <xdr:ext cx="6129694" cy="2028112"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -14338,7 +14538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -14547,10 +14747,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="A2" sqref="A2:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -14592,25 +14792,25 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="B2" s="7">
-        <v>0.91379999999999995</v>
+        <v>0.87609999999999999</v>
       </c>
       <c r="C2" s="7">
-        <v>0.53779999999999994</v>
+        <v>0.51449999999999996</v>
       </c>
       <c r="D2" s="7">
-        <v>0.75449999999999995</v>
+        <v>0.70809999999999995</v>
       </c>
       <c r="E2" s="7">
-        <v>0.98899999999999999</v>
+        <v>0.98219999999999996</v>
       </c>
       <c r="F2" s="7">
-        <v>0.96160000000000001</v>
+        <v>0.95250000000000001</v>
       </c>
       <c r="G2" s="7">
-        <v>0.58260000000000001</v>
+        <v>0.57750000000000001</v>
       </c>
       <c r="H2" s="7">
         <v>1</v>
@@ -14619,34 +14819,33 @@
         <v>0.9819</v>
       </c>
       <c r="J2" s="7">
-        <v>0.78669999999999995</v>
+        <v>0.77080000000000004</v>
       </c>
       <c r="K2" s="4">
-        <f>AVERAGE(B2:J2)</f>
-        <v>0.83421111111111101</v>
+        <v>0.81820000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B3" s="7">
-        <v>0.94740000000000002</v>
+        <v>0.91379999999999995</v>
       </c>
       <c r="C3" s="7">
-        <v>0.56659999999999999</v>
+        <v>0.53779999999999994</v>
       </c>
       <c r="D3" s="7">
-        <v>0.7843</v>
+        <v>0.75449999999999995</v>
       </c>
       <c r="E3" s="7">
-        <v>0.99690000000000001</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="F3" s="7">
-        <v>0.9647</v>
+        <v>0.96160000000000001</v>
       </c>
       <c r="G3" s="7">
-        <v>0.59370000000000001</v>
+        <v>0.58260000000000001</v>
       </c>
       <c r="H3" s="7">
         <v>1</v>
@@ -14655,34 +14854,33 @@
         <v>0.9819</v>
       </c>
       <c r="J3" s="7">
-        <v>0.80920000000000003</v>
+        <v>0.78669999999999995</v>
       </c>
       <c r="K3" s="4">
-        <f>AVERAGE(B3:J3)</f>
-        <v>0.84941111111111101</v>
+        <v>0.83420000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="7">
-        <v>0.98809999999999998</v>
+        <v>0.94740000000000002</v>
       </c>
       <c r="C4" s="7">
-        <v>0.61870000000000003</v>
+        <v>0.56659999999999999</v>
       </c>
       <c r="D4" s="7">
-        <v>0.84840000000000004</v>
+        <v>0.7843</v>
       </c>
       <c r="E4" s="7">
         <v>0.99690000000000001</v>
       </c>
       <c r="F4" s="7">
-        <v>0.97</v>
+        <v>0.9647</v>
       </c>
       <c r="G4" s="7">
-        <v>0.62849999999999995</v>
+        <v>0.59370000000000001</v>
       </c>
       <c r="H4" s="7">
         <v>1</v>
@@ -14691,70 +14889,68 @@
         <v>0.9819</v>
       </c>
       <c r="J4" s="7">
-        <v>0.84319999999999995</v>
+        <v>0.80920000000000003</v>
       </c>
       <c r="K4" s="4">
-        <f>AVERAGE(B4:J4)</f>
-        <v>0.87507777777777784</v>
+        <v>0.84940000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="7">
-        <v>1</v>
+        <v>0.98809999999999998</v>
       </c>
       <c r="C5" s="7">
-        <v>0.66549999999999998</v>
+        <v>0.61870000000000003</v>
       </c>
       <c r="D5" s="7">
-        <v>0.89729999999999999</v>
+        <v>0.84840000000000004</v>
       </c>
       <c r="E5" s="7">
-        <v>0.997</v>
+        <v>0.99690000000000001</v>
       </c>
       <c r="F5" s="7">
-        <v>0.97360000000000002</v>
+        <v>0.97</v>
       </c>
       <c r="G5" s="7">
-        <v>0.66720000000000002</v>
+        <v>0.62849999999999995</v>
       </c>
       <c r="H5" s="7">
         <v>1</v>
       </c>
       <c r="I5" s="7">
-        <v>0.98199999999999998</v>
+        <v>0.9819</v>
       </c>
       <c r="J5" s="7">
-        <v>0.87580000000000002</v>
+        <v>0.84319999999999995</v>
       </c>
       <c r="K5" s="4">
-        <f>AVERAGE(B5:J5)</f>
-        <v>0.89537777777777783</v>
+        <v>0.87509999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
       </c>
       <c r="C6" s="7">
-        <v>0.70620000000000005</v>
+        <v>0.66549999999999998</v>
       </c>
       <c r="D6" s="7">
-        <v>0.94279999999999997</v>
+        <v>0.89729999999999999</v>
       </c>
       <c r="E6" s="7">
         <v>0.997</v>
       </c>
       <c r="F6" s="7">
-        <v>0.97609999999999997</v>
+        <v>0.97360000000000002</v>
       </c>
       <c r="G6" s="7">
-        <v>0.65990000000000004</v>
+        <v>0.66720000000000002</v>
       </c>
       <c r="H6" s="7">
         <v>1</v>
@@ -14763,34 +14959,33 @@
         <v>0.98199999999999998</v>
       </c>
       <c r="J6" s="7">
-        <v>0.89590000000000003</v>
+        <v>0.87580000000000002</v>
       </c>
       <c r="K6" s="4">
-        <f>AVERAGE(B6:J6)</f>
-        <v>0.90665555555555555</v>
+        <v>0.89539999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="7">
         <v>1</v>
       </c>
       <c r="C7" s="7">
-        <v>0.73109999999999997</v>
+        <v>0.70620000000000005</v>
       </c>
       <c r="D7" s="7">
-        <v>0.98309999999999997</v>
+        <v>0.94279999999999997</v>
       </c>
       <c r="E7" s="7">
-        <v>0.99709999999999999</v>
+        <v>0.997</v>
       </c>
       <c r="F7" s="7">
-        <v>0.97909999999999997</v>
+        <v>0.97609999999999997</v>
       </c>
       <c r="G7" s="7">
-        <v>0.66790000000000005</v>
+        <v>0.65990000000000004</v>
       </c>
       <c r="H7" s="7">
         <v>1</v>
@@ -14799,34 +14994,33 @@
         <v>0.98199999999999998</v>
       </c>
       <c r="J7" s="7">
-        <v>0.95599999999999996</v>
+        <v>0.89590000000000003</v>
       </c>
       <c r="K7" s="4">
-        <f>AVERAGE(B7:J7)</f>
-        <v>0.92181111111111114</v>
+        <v>0.90669999999999995</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="7">
         <v>1</v>
       </c>
       <c r="C8" s="7">
-        <v>0.79949999999999999</v>
+        <v>0.73109999999999997</v>
       </c>
       <c r="D8" s="7">
-        <v>1</v>
+        <v>0.98309999999999997</v>
       </c>
       <c r="E8" s="7">
         <v>0.99709999999999999</v>
       </c>
       <c r="F8" s="7">
-        <v>0.98119999999999996</v>
+        <v>0.97909999999999997</v>
       </c>
       <c r="G8" s="7">
-        <v>0.74819999999999998</v>
+        <v>0.66790000000000005</v>
       </c>
       <c r="H8" s="7">
         <v>1</v>
@@ -14835,22 +15029,21 @@
         <v>0.98199999999999998</v>
       </c>
       <c r="J8" s="7">
-        <v>0.99439999999999995</v>
+        <v>0.95599999999999996</v>
       </c>
       <c r="K8" s="4">
-        <f>AVERAGE(B8:J8)</f>
-        <v>0.94471111111111106</v>
+        <v>0.92179999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" t="s">
-        <v>33</v>
+      <c r="A9" s="1">
+        <v>6</v>
       </c>
       <c r="B9" s="7">
         <v>1</v>
       </c>
       <c r="C9" s="7">
-        <v>0.86660000000000004</v>
+        <v>0.79949999999999999</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
@@ -14859,10 +15052,10 @@
         <v>0.99709999999999999</v>
       </c>
       <c r="F9" s="7">
-        <v>0.98319999999999996</v>
+        <v>0.98119999999999996</v>
       </c>
       <c r="G9" s="7">
-        <v>0.7742</v>
+        <v>0.74819999999999998</v>
       </c>
       <c r="H9" s="7">
         <v>1</v>
@@ -14871,11 +15064,45 @@
         <v>0.98199999999999998</v>
       </c>
       <c r="J9" s="7">
+        <v>0.99439999999999995</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0.94469999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0.86660000000000004</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.99709999999999999</v>
+      </c>
+      <c r="F10">
+        <v>0.98319999999999996</v>
+      </c>
+      <c r="G10">
+        <v>0.7742</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="J10">
         <v>0.99970000000000003</v>
       </c>
-      <c r="K9" s="4">
-        <f>AVERAGE(B9:J9)</f>
-        <v>0.95586666666666664</v>
+      <c r="K10">
+        <v>0.95589999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -14891,10 +15118,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection sqref="A1:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -14905,231 +15132,226 @@
     <row r="1" spans="1:11">
       <c r="A1" s="2"/>
       <c r="B1" s="6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="B2" s="7">
-        <v>0.43049999999999999</v>
+        <v>0.26540000000000002</v>
       </c>
       <c r="C2" s="7">
-        <v>0.22689999999999999</v>
+        <v>0.10780000000000001</v>
       </c>
       <c r="D2" s="7">
-        <v>0.44140000000000001</v>
+        <v>0.27150000000000002</v>
       </c>
       <c r="E2" s="7">
-        <v>0.82330000000000003</v>
+        <v>0.34770000000000001</v>
       </c>
       <c r="F2" s="7">
-        <v>0.39529999999999998</v>
+        <v>0.2445</v>
       </c>
       <c r="G2" s="7">
-        <v>0.4148</v>
+        <v>0.12690000000000001</v>
       </c>
       <c r="H2" s="7">
-        <v>0.49149999999999999</v>
+        <v>0.36809999999999998</v>
       </c>
       <c r="I2" s="7">
-        <v>0.97660000000000002</v>
+        <v>0.9587</v>
       </c>
       <c r="J2" s="7">
-        <v>0.3533</v>
+        <v>0.1996</v>
       </c>
       <c r="K2" s="4">
-        <f>AVERAGE(B2:J2)</f>
-        <v>0.5059555555555556</v>
+        <v>0.3211</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B3" s="7">
-        <v>0.55300000000000005</v>
+        <v>0.43049999999999999</v>
       </c>
       <c r="C3" s="7">
-        <v>0.32629999999999998</v>
+        <v>0.22689999999999999</v>
       </c>
       <c r="D3" s="7">
-        <v>0.59430000000000005</v>
+        <v>0.44140000000000001</v>
       </c>
       <c r="E3" s="7">
-        <v>0.89680000000000004</v>
+        <v>0.82330000000000003</v>
       </c>
       <c r="F3" s="7">
-        <v>0.51849999999999996</v>
+        <v>0.39529999999999998</v>
       </c>
       <c r="G3" s="7">
-        <v>0.74660000000000004</v>
+        <v>0.4148</v>
       </c>
       <c r="H3" s="7">
-        <v>0.59719999999999995</v>
+        <v>0.49149999999999999</v>
       </c>
       <c r="I3" s="7">
-        <v>0.99470000000000003</v>
+        <v>0.97660000000000002</v>
       </c>
       <c r="J3" s="7">
-        <v>0.47570000000000001</v>
+        <v>0.3533</v>
       </c>
       <c r="K3" s="4">
-        <f>AVERAGE(B3:J3)</f>
-        <v>0.63367777777777767</v>
+        <v>0.50600000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="7">
-        <v>0.78580000000000005</v>
+        <v>0.55300000000000005</v>
       </c>
       <c r="C4" s="7">
-        <v>0.51400000000000001</v>
+        <v>0.32629999999999998</v>
       </c>
       <c r="D4" s="7">
-        <v>0.81979999999999997</v>
+        <v>0.59430000000000005</v>
       </c>
       <c r="E4" s="7">
-        <v>0.94910000000000005</v>
+        <v>0.89680000000000004</v>
       </c>
       <c r="F4" s="7">
-        <v>0.70230000000000004</v>
+        <v>0.51849999999999996</v>
       </c>
       <c r="G4" s="7">
-        <v>0.91339999999999999</v>
+        <v>0.74660000000000004</v>
       </c>
       <c r="H4" s="7">
-        <v>0.8196</v>
+        <v>0.59719999999999995</v>
       </c>
       <c r="I4" s="7">
-        <v>0.99860000000000004</v>
+        <v>0.99470000000000003</v>
       </c>
       <c r="J4" s="7">
-        <v>0.71289999999999998</v>
+        <v>0.47570000000000001</v>
       </c>
       <c r="K4" s="4">
-        <f>AVERAGE(B4:J4)</f>
-        <v>0.80172222222222222</v>
+        <v>0.63370000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="7">
-        <v>1</v>
+        <v>0.78580000000000005</v>
       </c>
       <c r="C5" s="7">
-        <v>0.64870000000000005</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="D5" s="7">
-        <v>0.99650000000000005</v>
+        <v>0.81979999999999997</v>
       </c>
       <c r="E5" s="7">
-        <v>0.98370000000000002</v>
+        <v>0.94910000000000005</v>
       </c>
       <c r="F5" s="7">
-        <v>0.86770000000000003</v>
+        <v>0.70230000000000004</v>
       </c>
       <c r="G5" s="7">
-        <v>1</v>
+        <v>0.91339999999999999</v>
       </c>
       <c r="H5" s="7">
-        <v>0.99839999999999995</v>
+        <v>0.8196</v>
       </c>
       <c r="I5" s="7">
-        <v>0.99960000000000004</v>
+        <v>0.99860000000000004</v>
       </c>
       <c r="J5" s="7">
-        <v>0.9284</v>
+        <v>0.71289999999999998</v>
       </c>
       <c r="K5" s="4">
-        <f>AVERAGE(B5:J5)</f>
-        <v>0.93588888888888888</v>
+        <v>0.80169999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
       </c>
       <c r="C6" s="7">
-        <v>0.77729999999999999</v>
+        <v>0.64870000000000005</v>
       </c>
       <c r="D6" s="7">
-        <v>1</v>
+        <v>0.99650000000000005</v>
       </c>
       <c r="E6" s="7">
-        <v>0.99980000000000002</v>
+        <v>0.98370000000000002</v>
       </c>
       <c r="F6" s="7">
-        <v>1</v>
+        <v>0.86770000000000003</v>
       </c>
       <c r="G6" s="7">
         <v>1</v>
       </c>
       <c r="H6" s="7">
-        <v>0.99919999999999998</v>
+        <v>0.99839999999999995</v>
       </c>
       <c r="I6" s="7">
-        <v>0.99980000000000002</v>
+        <v>0.99960000000000004</v>
       </c>
       <c r="J6" s="7">
-        <v>1</v>
+        <v>0.9284</v>
       </c>
       <c r="K6" s="4">
-        <f>AVERAGE(B6:J6)</f>
-        <v>0.97512222222222222</v>
+        <v>0.93589999999999995</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="7">
         <v>1</v>
       </c>
       <c r="C7" s="7">
-        <v>0.91</v>
+        <v>0.77729999999999999</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
       </c>
       <c r="E7" s="7">
-        <v>0.99990000000000001</v>
+        <v>0.99980000000000002</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
@@ -15138,28 +15360,27 @@
         <v>1</v>
       </c>
       <c r="H7" s="7">
-        <v>0.99929999999999997</v>
+        <v>0.99919999999999998</v>
       </c>
       <c r="I7" s="7">
-        <v>1</v>
+        <v>0.99980000000000002</v>
       </c>
       <c r="J7" s="7">
         <v>1</v>
       </c>
       <c r="K7" s="4">
-        <f>AVERAGE(B7:J7)</f>
-        <v>0.98991111111111119</v>
+        <v>0.97509999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="7">
         <v>1</v>
       </c>
       <c r="C8" s="7">
-        <v>0.99199999999999999</v>
+        <v>0.91</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
@@ -15174,7 +15395,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="7">
-        <v>0.99939999999999996</v>
+        <v>0.99929999999999997</v>
       </c>
       <c r="I8" s="7">
         <v>1</v>
@@ -15183,25 +15404,24 @@
         <v>1</v>
       </c>
       <c r="K8" s="4">
-        <f>AVERAGE(B8:J8)</f>
-        <v>0.99903333333333322</v>
+        <v>0.9899</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="2" t="s">
-        <v>33</v>
+      <c r="A9" s="1">
+        <v>6</v>
       </c>
       <c r="B9" s="7">
         <v>1</v>
       </c>
       <c r="C9" s="7">
-        <v>1</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
       </c>
       <c r="E9" s="7">
-        <v>1</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="F9" s="7">
         <v>1</v>
@@ -15219,8 +15439,42 @@
         <v>1</v>
       </c>
       <c r="K9" s="4">
-        <f>AVERAGE(B9:J9)</f>
-        <v>0.99993333333333334</v>
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0.99939999999999996</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0.99990000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor edits to evalutation.
</commit_message>
<xml_diff>
--- a/figs_src/data.xlsx
+++ b/figs_src/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" checkCompatibility="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17475" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17475" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="full_mon" sheetId="1" r:id="rId1"/>
@@ -4717,6 +4717,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0_);[Red]\(0.0\)" sourceLinked="1"/>
@@ -6827,8 +6828,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.20591144795083699"/>
           <c:y val="0.84352873660022498"/>
-          <c:w val="0.65846255946871091"/>
-          <c:h val="9.2497357147928713E-2"/>
+          <c:w val="0.6423086850840265"/>
+          <c:h val="8.5941855761350147E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -12051,7 +12052,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="147" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="144" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="159" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -12258,7 +12259,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="3075653" cy="2175387"/>
+    <xdr:ext cx="2925097" cy="2021758"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1"/>
@@ -12312,7 +12313,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="6129694" cy="2028112"/>
+    <xdr:ext cx="6283854" cy="2182813"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -14536,10 +14537,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -14732,6 +14733,23 @@
       <c r="K8" s="2">
         <f>0.5/(K3-1)</f>
         <v>0.20215007350133049</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="K9" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="K10" s="2">
+        <f>0.1/K2</f>
+        <v>2.8423119377468317E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="K11" s="2">
+        <f>0.1/K3</f>
+        <v>2.8790152010280672E-2</v>
       </c>
     </row>
   </sheetData>
@@ -15120,7 +15138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:K10"/>
     </sheetView>
   </sheetViews>

</xml_diff>